<commit_message>
added grades and copo for cse 208 section 1 & section 2
</commit_message>
<xml_diff>
--- a/FALL 19/CSE 208/results_cse208_sec2.xlsx
+++ b/FALL 19/CSE 208/results_cse208_sec2.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A972BE1A-2922-4063-9CD9-9AC9AA537BA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="21840" windowHeight="13740" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attendance" sheetId="6" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId8"/>
   </externalReferences>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -222,8 +223,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,7 +462,7 @@
   <cellStyles count="3">
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="20">
     <dxf>
@@ -680,7 +681,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1230,7 +1231,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1262,9 +1263,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1296,6 +1315,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1471,22 +1508,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="16" customWidth="1"/>
-    <col min="3" max="8" width="14.7109375" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="14.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="16" customWidth="1"/>
+    <col min="3" max="8" width="14.6640625" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1512,7 +1549,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>153014012</v>
       </c>
@@ -1542,7 +1579,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>171014081</v>
       </c>
@@ -1572,7 +1609,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>173014009</v>
       </c>
@@ -1602,7 +1639,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>173014029</v>
       </c>
@@ -1632,7 +1669,7 @@
         <v>A-</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>181014002</v>
       </c>
@@ -1662,7 +1699,7 @@
         <v>A-</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>181014008</v>
       </c>
@@ -1692,7 +1729,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>181014025</v>
       </c>
@@ -1722,7 +1759,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>181014032</v>
       </c>
@@ -1752,7 +1789,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>181014057</v>
       </c>
@@ -1782,7 +1819,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>181014060</v>
       </c>
@@ -1812,7 +1849,7 @@
         <v>A-</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>181014131</v>
       </c>
@@ -1842,7 +1879,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>182014030</v>
       </c>
@@ -1872,7 +1909,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>182014052</v>
       </c>
@@ -1902,7 +1939,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>182014055</v>
       </c>
@@ -1932,7 +1969,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>182014061</v>
       </c>
@@ -1962,7 +1999,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>182014069</v>
       </c>
@@ -1992,7 +2029,7 @@
         <v>A-</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>182014071</v>
       </c>
@@ -2022,7 +2059,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>183014002</v>
       </c>
@@ -2052,7 +2089,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>183014004</v>
       </c>
@@ -2082,7 +2119,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>183014007</v>
       </c>
@@ -2112,7 +2149,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>183014009</v>
       </c>
@@ -2142,7 +2179,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>183014012</v>
       </c>
@@ -2172,7 +2209,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>183014014</v>
       </c>
@@ -2202,7 +2239,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>183014017</v>
       </c>
@@ -2232,7 +2269,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>183014024</v>
       </c>
@@ -2262,7 +2299,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>183014029</v>
       </c>
@@ -2292,7 +2329,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>183014031</v>
       </c>
@@ -2322,7 +2359,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>183014035</v>
       </c>
@@ -2352,7 +2389,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>183014046</v>
       </c>
@@ -2382,7 +2419,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>183014050</v>
       </c>
@@ -2412,7 +2449,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>183014052</v>
       </c>
@@ -2442,7 +2479,7 @@
         <v>A-</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>183014056</v>
       </c>
@@ -2472,7 +2509,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>183014057</v>
       </c>
@@ -2502,7 +2539,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>183014063</v>
       </c>
@@ -2532,7 +2569,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1">
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>183014073</v>
       </c>
@@ -2562,7 +2599,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F37" s="16">
         <v>10</v>
       </c>
@@ -2583,22 +2620,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
-    <col min="3" max="12" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="12" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.95" customHeight="1">
+    <row r="1" spans="1:12" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2636,7 +2673,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>153014012</v>
       </c>
@@ -2678,7 +2715,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>171014081</v>
       </c>
@@ -2714,7 +2751,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>173014009</v>
       </c>
@@ -2756,7 +2793,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>173014029</v>
       </c>
@@ -2798,7 +2835,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1">
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>181014002</v>
       </c>
@@ -2840,7 +2877,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1">
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>181014008</v>
       </c>
@@ -2876,7 +2913,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1">
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>181014025</v>
       </c>
@@ -2912,7 +2949,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>181014032</v>
       </c>
@@ -2948,7 +2985,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1">
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>181014057</v>
       </c>
@@ -2984,7 +3021,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1">
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>181014060</v>
       </c>
@@ -3026,7 +3063,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1">
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>181014131</v>
       </c>
@@ -3062,7 +3099,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1">
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>182014030</v>
       </c>
@@ -3098,7 +3135,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1">
+    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>182014052</v>
       </c>
@@ -3140,7 +3177,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" customHeight="1">
+    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>182014055</v>
       </c>
@@ -3182,7 +3219,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1">
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>182014061</v>
       </c>
@@ -3218,7 +3255,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" customHeight="1">
+    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>182014069</v>
       </c>
@@ -3260,7 +3297,7 @@
         <v>A-</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15" customHeight="1">
+    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>182014071</v>
       </c>
@@ -3302,7 +3339,7 @@
         <v>B-</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" customHeight="1">
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>183014002</v>
       </c>
@@ -3344,7 +3381,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" customHeight="1">
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>183014004</v>
       </c>
@@ -3386,7 +3423,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15" customHeight="1">
+    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>183014007</v>
       </c>
@@ -3428,7 +3465,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1">
+    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>183014009</v>
       </c>
@@ -3464,7 +3501,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" customHeight="1">
+    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>183014012</v>
       </c>
@@ -3506,7 +3543,7 @@
         <v>A-</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15" customHeight="1">
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>183014014</v>
       </c>
@@ -3548,7 +3585,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15" customHeight="1">
+    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>183014017</v>
       </c>
@@ -3590,7 +3627,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15" customHeight="1">
+    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>183014024</v>
       </c>
@@ -3632,7 +3669,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15" customHeight="1">
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>183014029</v>
       </c>
@@ -3668,7 +3705,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15" customHeight="1">
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>183014031</v>
       </c>
@@ -3710,7 +3747,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15" customHeight="1">
+    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>183014035</v>
       </c>
@@ -3752,7 +3789,7 @@
         <v>C</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1">
+    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>183014046</v>
       </c>
@@ -3794,7 +3831,7 @@
         <v>B-</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15" customHeight="1">
+    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>183014050</v>
       </c>
@@ -3836,7 +3873,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15" customHeight="1">
+    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>183014052</v>
       </c>
@@ -3872,7 +3909,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15" customHeight="1">
+    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>183014056</v>
       </c>
@@ -3914,7 +3951,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15" customHeight="1">
+    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>183014057</v>
       </c>
@@ -3956,7 +3993,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15" customHeight="1">
+    <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>183014063</v>
       </c>
@@ -3998,7 +4035,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1" thickBot="1">
+    <row r="36" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>183014073</v>
       </c>
@@ -4067,21 +4104,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="10" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="10" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4113,7 +4150,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>153014012</v>
       </c>
@@ -4147,7 +4184,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>171014081</v>
       </c>
@@ -4179,7 +4216,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>173014009</v>
       </c>
@@ -4211,7 +4248,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>173014029</v>
       </c>
@@ -4247,7 +4284,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>181014002</v>
       </c>
@@ -4283,7 +4320,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>181014008</v>
       </c>
@@ -4315,7 +4352,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>181014025</v>
       </c>
@@ -4351,7 +4388,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>181014032</v>
       </c>
@@ -4385,7 +4422,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>181014057</v>
       </c>
@@ -4421,7 +4458,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>181014060</v>
       </c>
@@ -4457,7 +4494,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>181014131</v>
       </c>
@@ -4489,7 +4526,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>182014030</v>
       </c>
@@ -4525,7 +4562,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>182014052</v>
       </c>
@@ -4561,7 +4598,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>182014055</v>
       </c>
@@ -4597,7 +4634,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>182014061</v>
       </c>
@@ -4629,7 +4666,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>182014069</v>
       </c>
@@ -4665,7 +4702,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>182014071</v>
       </c>
@@ -4701,7 +4738,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>183014002</v>
       </c>
@@ -4737,7 +4774,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>183014004</v>
       </c>
@@ -4773,7 +4810,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>183014007</v>
       </c>
@@ -4809,7 +4846,7 @@
         <v>A-</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>183014009</v>
       </c>
@@ -4845,7 +4882,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>183014012</v>
       </c>
@@ -4881,7 +4918,7 @@
         <v>B+</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>183014014</v>
       </c>
@@ -4917,7 +4954,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>183014017</v>
       </c>
@@ -4953,7 +4990,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>183014024</v>
       </c>
@@ -4989,7 +5026,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>183014029</v>
       </c>
@@ -5021,7 +5058,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>183014031</v>
       </c>
@@ -5057,7 +5094,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>183014035</v>
       </c>
@@ -5093,7 +5130,7 @@
         <v>B-</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>183014046</v>
       </c>
@@ -5129,7 +5166,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>183014050</v>
       </c>
@@ -5165,7 +5202,7 @@
         <v>B-</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>183014052</v>
       </c>
@@ -5201,7 +5238,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>183014056</v>
       </c>
@@ -5237,7 +5274,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>183014057</v>
       </c>
@@ -5273,7 +5310,7 @@
         <v>B-</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>183014063</v>
       </c>
@@ -5309,7 +5346,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1">
+    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>183014073</v>
       </c>
@@ -5366,21 +5403,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="12" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="29" customFormat="1">
+    <row r="1" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -5418,7 +5455,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>153014012</v>
       </c>
@@ -5461,7 +5498,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>171014081</v>
       </c>
@@ -5504,7 +5541,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>173014009</v>
       </c>
@@ -5547,7 +5584,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>173014029</v>
       </c>
@@ -5590,7 +5627,7 @@
         <v>B-</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>181014002</v>
       </c>
@@ -5633,7 +5670,7 @@
         <v>B-</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>181014008</v>
       </c>
@@ -5676,7 +5713,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>181014025</v>
       </c>
@@ -5719,7 +5756,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>181014032</v>
       </c>
@@ -5762,7 +5799,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>181014057</v>
       </c>
@@ -5805,7 +5842,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>181014060</v>
       </c>
@@ -5848,7 +5885,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>181014131</v>
       </c>
@@ -5891,7 +5928,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>182014030</v>
       </c>
@@ -5934,7 +5971,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>182014052</v>
       </c>
@@ -5977,7 +6014,7 @@
         <v>C</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>182014055</v>
       </c>
@@ -6020,7 +6057,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>182014061</v>
       </c>
@@ -6063,7 +6100,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>182014069</v>
       </c>
@@ -6106,7 +6143,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>182014071</v>
       </c>
@@ -6149,7 +6186,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>183014002</v>
       </c>
@@ -6192,7 +6229,7 @@
         <v>B+</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>183014004</v>
       </c>
@@ -6235,7 +6272,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>183014007</v>
       </c>
@@ -6278,7 +6315,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>183014009</v>
       </c>
@@ -6321,7 +6358,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>183014012</v>
       </c>
@@ -6364,7 +6401,7 @@
         <v>B+</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>183014014</v>
       </c>
@@ -6407,7 +6444,7 @@
         <v>C</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>183014017</v>
       </c>
@@ -6450,7 +6487,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>183014024</v>
       </c>
@@ -6493,7 +6530,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>183014029</v>
       </c>
@@ -6536,7 +6573,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>183014031</v>
       </c>
@@ -6579,7 +6616,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>183014035</v>
       </c>
@@ -6622,7 +6659,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>183014046</v>
       </c>
@@ -6665,7 +6702,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>183014050</v>
       </c>
@@ -6708,7 +6745,7 @@
         <v>A-</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>183014052</v>
       </c>
@@ -6751,7 +6788,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>183014056</v>
       </c>
@@ -6794,7 +6831,7 @@
         <v>A-</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>183014057</v>
       </c>
@@ -6837,7 +6874,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>183014063</v>
       </c>
@@ -6880,7 +6917,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" thickBot="1">
+    <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>183014073</v>
       </c>
@@ -6923,23 +6960,23 @@
         <v>F</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="K37" s="18"/>
       <c r="L37" s="21"/>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="K38" s="18"/>
       <c r="L38" s="21"/>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="K39" s="19"/>
       <c r="L39" s="21"/>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="K40" s="19"/>
       <c r="L40" s="21"/>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
       <c r="I41" s="16"/>
@@ -6959,22 +6996,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:N36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="13" width="14.7109375" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="13" width="14.6640625" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.95" customHeight="1">
+    <row r="1" spans="1:14" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -7018,7 +7055,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1">
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>153014012</v>
       </c>
@@ -7062,7 +7099,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>171014081</v>
       </c>
@@ -7102,7 +7139,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>173014009</v>
       </c>
@@ -7146,7 +7183,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>173014029</v>
       </c>
@@ -7192,7 +7229,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>181014002</v>
       </c>
@@ -7238,7 +7275,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>181014008</v>
       </c>
@@ -7284,7 +7321,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>181014025</v>
       </c>
@@ -7330,7 +7367,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>181014032</v>
       </c>
@@ -7372,7 +7409,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>181014057</v>
       </c>
@@ -7418,7 +7455,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>181014060</v>
       </c>
@@ -7462,7 +7499,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>181014131</v>
       </c>
@@ -7506,7 +7543,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>182014030</v>
       </c>
@@ -7550,7 +7587,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>182014052</v>
       </c>
@@ -7594,7 +7631,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>182014055</v>
       </c>
@@ -7640,7 +7677,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>182014061</v>
       </c>
@@ -7686,7 +7723,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>182014069</v>
       </c>
@@ -7730,7 +7767,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>182014071</v>
       </c>
@@ -7774,7 +7811,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>183014002</v>
       </c>
@@ -7822,7 +7859,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>183014004</v>
       </c>
@@ -7866,7 +7903,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>183014007</v>
       </c>
@@ -7910,7 +7947,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>183014009</v>
       </c>
@@ -7954,7 +7991,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>183014012</v>
       </c>
@@ -8000,7 +8037,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>183014014</v>
       </c>
@@ -8046,7 +8083,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>183014017</v>
       </c>
@@ -8090,7 +8127,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>183014024</v>
       </c>
@@ -8134,7 +8171,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>183014029</v>
       </c>
@@ -8178,7 +8215,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>183014031</v>
       </c>
@@ -8224,7 +8261,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>183014035</v>
       </c>
@@ -8270,7 +8307,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>183014046</v>
       </c>
@@ -8316,7 +8353,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>183014050</v>
       </c>
@@ -8360,7 +8397,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>183014052</v>
       </c>
@@ -8406,7 +8443,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>183014056</v>
       </c>
@@ -8452,7 +8489,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>183014057</v>
       </c>
@@ -8496,7 +8533,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>183014063</v>
       </c>
@@ -8542,7 +8579,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1">
+    <row r="36" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>183014073</v>
       </c>
@@ -8618,21 +8655,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="14" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="14" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8676,7 +8713,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>153014012</v>
       </c>
@@ -8720,7 +8757,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>171014081</v>
       </c>
@@ -8760,7 +8797,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>173014009</v>
       </c>
@@ -8800,7 +8837,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>173014029</v>
       </c>
@@ -8846,7 +8883,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>181014002</v>
       </c>
@@ -8894,7 +8931,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>181014008</v>
       </c>
@@ -8934,7 +8971,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>181014025</v>
       </c>
@@ -8978,7 +9015,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>181014032</v>
       </c>
@@ -9018,7 +9055,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>181014057</v>
       </c>
@@ -9058,7 +9095,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>181014060</v>
       </c>
@@ -9106,7 +9143,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>181014131</v>
       </c>
@@ -9146,7 +9183,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>182014030</v>
       </c>
@@ -9192,7 +9229,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>182014052</v>
       </c>
@@ -9236,7 +9273,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>182014055</v>
       </c>
@@ -9284,7 +9321,7 @@
         <v>C</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>182014061</v>
       </c>
@@ -9324,7 +9361,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>182014069</v>
       </c>
@@ -9364,7 +9401,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>182014071</v>
       </c>
@@ -9404,7 +9441,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>183014002</v>
       </c>
@@ -9452,7 +9489,7 @@
         <v>B+</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>183014004</v>
       </c>
@@ -9496,7 +9533,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>183014007</v>
       </c>
@@ -9544,7 +9581,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>183014009</v>
       </c>
@@ -9592,7 +9629,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>183014012</v>
       </c>
@@ -9636,7 +9673,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>183014014</v>
       </c>
@@ -9684,7 +9721,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>183014017</v>
       </c>
@@ -9732,7 +9769,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>183014024</v>
       </c>
@@ -9780,7 +9817,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>183014029</v>
       </c>
@@ -9820,7 +9857,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>183014031</v>
       </c>
@@ -9868,7 +9905,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>183014035</v>
       </c>
@@ -9916,7 +9953,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>183014046</v>
       </c>
@@ -9960,7 +9997,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>183014050</v>
       </c>
@@ -10008,7 +10045,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>183014052</v>
       </c>
@@ -10056,7 +10093,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>183014056</v>
       </c>
@@ -10100,7 +10137,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>183014057</v>
       </c>
@@ -10148,7 +10185,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>183014063</v>
       </c>
@@ -10196,7 +10233,7 @@
         <v>C</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1">
+    <row r="36" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>183014073</v>
       </c>
@@ -10275,22 +10312,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="16" customWidth="1"/>
-    <col min="3" max="7" width="14.7109375" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="14.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" style="16" customWidth="1"/>
+    <col min="3" max="7" width="14.6640625" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -10313,7 +10350,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>153014012</v>
       </c>
@@ -10333,15 +10370,15 @@
         <v>12</v>
       </c>
       <c r="F2" s="33">
-        <f>(E2/E$37)*100</f>
+        <f t="shared" ref="F2:F36" si="1">(E2/E$37)*100</f>
         <v>60</v>
       </c>
       <c r="G2" s="34" t="str">
-        <f t="shared" ref="G2:G36" si="1">IF(F2&gt;94,"A+",IF(F2&gt;84,"A",IF(F2&gt;79,"A-",IF(F2&gt;74,"B+",IF(F2&gt;69,"B",IF(F2&gt;64,"B-",IF(F2&gt;59,"C+",IF(F2&gt;54,"C",IF(F2&gt;49,"D","F")))))))))</f>
+        <f t="shared" ref="G2:G36" si="2">IF(F2&gt;94,"A+",IF(F2&gt;84,"A",IF(F2&gt;79,"A-",IF(F2&gt;74,"B+",IF(F2&gt;69,"B",IF(F2&gt;64,"B-",IF(F2&gt;59,"C+",IF(F2&gt;54,"C",IF(F2&gt;49,"D","F")))))))))</f>
         <v>C+</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>171014081</v>
       </c>
@@ -10361,15 +10398,15 @@
         <v>12</v>
       </c>
       <c r="F3" s="33">
-        <f>(E3/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="G3" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C+</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>173014009</v>
       </c>
@@ -10389,15 +10426,15 @@
         <v>19</v>
       </c>
       <c r="F4" s="33">
-        <f>(E4/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="G4" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A+</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>173014029</v>
       </c>
@@ -10417,15 +10454,15 @@
         <v>14</v>
       </c>
       <c r="F5" s="33">
-        <f>(E5/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="G5" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>181014002</v>
       </c>
@@ -10445,15 +10482,15 @@
         <v>17</v>
       </c>
       <c r="F6" s="33">
-        <f>(E6/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="G6" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>181014008</v>
       </c>
@@ -10473,15 +10510,15 @@
         <v>14</v>
       </c>
       <c r="F7" s="33">
-        <f>(E7/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="G7" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>181014025</v>
       </c>
@@ -10501,15 +10538,15 @@
         <v>12</v>
       </c>
       <c r="F8" s="33">
-        <f>(E8/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="G8" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C+</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>181014032</v>
       </c>
@@ -10529,15 +10566,15 @@
         <v>17.5</v>
       </c>
       <c r="F9" s="33">
-        <f>(E9/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>87.5</v>
       </c>
       <c r="G9" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>181014057</v>
       </c>
@@ -10557,15 +10594,15 @@
         <v>12</v>
       </c>
       <c r="F10" s="33">
-        <f>(E10/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="G10" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C+</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>181014060</v>
       </c>
@@ -10585,15 +10622,15 @@
         <v>12</v>
       </c>
       <c r="F11" s="33">
-        <f>(E11/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="G11" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C+</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>181014131</v>
       </c>
@@ -10613,15 +10650,15 @@
         <v>18.5</v>
       </c>
       <c r="F12" s="33">
-        <f>(E12/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>92.5</v>
       </c>
       <c r="G12" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>182014030</v>
       </c>
@@ -10641,15 +10678,15 @@
         <v>12</v>
       </c>
       <c r="F13" s="33">
-        <f>(E13/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="G13" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C+</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>182014052</v>
       </c>
@@ -10669,15 +10706,15 @@
         <v>18</v>
       </c>
       <c r="F14" s="33">
-        <f>(E14/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="G14" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>182014055</v>
       </c>
@@ -10697,15 +10734,15 @@
         <v>17</v>
       </c>
       <c r="F15" s="33">
-        <f>(E15/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="G15" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>182014061</v>
       </c>
@@ -10725,15 +10762,15 @@
         <v>18</v>
       </c>
       <c r="F16" s="33">
-        <f>(E16/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="G16" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>182014069</v>
       </c>
@@ -10753,15 +10790,15 @@
         <v>17.5</v>
       </c>
       <c r="F17" s="33">
-        <f>(E17/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>87.5</v>
       </c>
       <c r="G17" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>182014071</v>
       </c>
@@ -10781,15 +10818,15 @@
         <v>12</v>
       </c>
       <c r="F18" s="33">
-        <f>(E18/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="G18" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C+</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>183014002</v>
       </c>
@@ -10809,15 +10846,15 @@
         <v>19</v>
       </c>
       <c r="F19" s="33">
-        <f>(E19/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="G19" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A+</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>183014004</v>
       </c>
@@ -10837,15 +10874,15 @@
         <v>19</v>
       </c>
       <c r="F20" s="33">
-        <f>(E20/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="G20" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A+</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>183014007</v>
       </c>
@@ -10865,15 +10902,15 @@
         <v>19</v>
       </c>
       <c r="F21" s="33">
-        <f>(E21/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="G21" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A+</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>183014009</v>
       </c>
@@ -10893,15 +10930,15 @@
         <v>18.5</v>
       </c>
       <c r="F22" s="33">
-        <f>(E22/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>92.5</v>
       </c>
       <c r="G22" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>183014012</v>
       </c>
@@ -10921,15 +10958,15 @@
         <v>19</v>
       </c>
       <c r="F23" s="33">
-        <f>(E23/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="G23" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A+</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>183014014</v>
       </c>
@@ -10949,15 +10986,15 @@
         <v>17</v>
       </c>
       <c r="F24" s="33">
-        <f>(E24/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="G24" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>183014017</v>
       </c>
@@ -10977,15 +11014,15 @@
         <v>17.5</v>
       </c>
       <c r="F25" s="33">
-        <f>(E25/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>87.5</v>
       </c>
       <c r="G25" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>183014024</v>
       </c>
@@ -11005,15 +11042,15 @@
         <v>14</v>
       </c>
       <c r="F26" s="33">
-        <f>(E26/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="G26" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>183014029</v>
       </c>
@@ -11033,15 +11070,15 @@
         <v>19</v>
       </c>
       <c r="F27" s="33">
-        <f>(E27/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="G27" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A+</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>183014031</v>
       </c>
@@ -11061,15 +11098,15 @@
         <v>18</v>
       </c>
       <c r="F28" s="33">
-        <f>(E28/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="G28" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>183014035</v>
       </c>
@@ -11089,15 +11126,15 @@
         <v>17.5</v>
       </c>
       <c r="F29" s="33">
-        <f>(E29/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>87.5</v>
       </c>
       <c r="G29" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>183014046</v>
       </c>
@@ -11117,15 +11154,15 @@
         <v>18.5</v>
       </c>
       <c r="F30" s="33">
-        <f>(E30/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>92.5</v>
       </c>
       <c r="G30" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>183014050</v>
       </c>
@@ -11145,15 +11182,15 @@
         <v>19</v>
       </c>
       <c r="F31" s="33">
-        <f>(E31/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="G31" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A+</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>183014052</v>
       </c>
@@ -11173,15 +11210,15 @@
         <v>17</v>
       </c>
       <c r="F32" s="33">
-        <f>(E32/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="G32" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>183014056</v>
       </c>
@@ -11201,15 +11238,15 @@
         <v>17</v>
       </c>
       <c r="F33" s="33">
-        <f>(E33/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="G33" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>183014057</v>
       </c>
@@ -11229,15 +11266,15 @@
         <v>17.5</v>
       </c>
       <c r="F34" s="33">
-        <f>(E34/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>87.5</v>
       </c>
       <c r="G34" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>183014063</v>
       </c>
@@ -11257,15 +11294,15 @@
         <v>17</v>
       </c>
       <c r="F35" s="33">
-        <f>(E35/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="G35" s="34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1">
+    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>183014073</v>
       </c>
@@ -11285,15 +11322,15 @@
         <v>17.5</v>
       </c>
       <c r="F36" s="35">
-        <f>(E36/E$37)*100</f>
+        <f t="shared" si="1"/>
         <v>87.5</v>
       </c>
       <c r="G36" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C37" s="16">
         <v>10</v>
       </c>

</xml_diff>